<commit_message>
added more test cases for Airbnb
</commit_message>
<xml_diff>
--- a/com.airbnb/src/test/resources/testData/placesToStayTestData.xlsx
+++ b/com.airbnb/src/test/resources/testData/placesToStayTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>location</t>
   </si>
@@ -30,10 +30,28 @@
     <t>Seattle</t>
   </si>
   <si>
-    <t xml:space="preserve"> 12/10/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12/16/2021</t>
+    <t xml:space="preserve"> 09/10/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/16/2022</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12/12/2021</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12/25/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/30/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9/28/2021</t>
   </si>
 </sst>
 </file>
@@ -373,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,6 +425,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added more DDT test cases for BoA
</commit_message>
<xml_diff>
--- a/com.airbnb/src/test/resources/testData/placesToStayTestData.xlsx
+++ b/com.airbnb/src/test/resources/testData/placesToStayTestData.xlsx
@@ -30,12 +30,6 @@
     <t>Seattle</t>
   </si>
   <si>
-    <t xml:space="preserve"> 09/10/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11/16/2022</t>
-  </si>
-  <si>
     <t>Los Angeles</t>
   </si>
   <si>
@@ -45,13 +39,19 @@
     <t xml:space="preserve"> 12/25/2021</t>
   </si>
   <si>
-    <t xml:space="preserve"> 11/30/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9/28/2021</t>
-  </si>
-  <si>
     <t>Kansas City</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/15/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02/15/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01/05/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02/19/2022</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -419,32 +419,32 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>